<commit_message>
Modified controller parameters, factor in front tyre camber stiffness
</commit_message>
<xml_diff>
--- a/Data/Data.xlsx
+++ b/Data/Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20367"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ga53hon\Desktop\motorcycle_model\Daten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ga53hon\Desktop\Motorcycle_Dirk_201028\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00A4B2E-6613-43A5-8031-C6822FB43A28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24240" yWindow="240" windowWidth="21600" windowHeight="11388" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Geometry" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="Tire" sheetId="2" r:id="rId3"/>
     <sheet name="Stiffness" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="165">
   <si>
     <t>Group_Frame</t>
   </si>
@@ -191,9 +192,6 @@
     <t>r_rim_FW</t>
   </si>
   <si>
-    <t>Fz0_FW</t>
-  </si>
-  <si>
     <t>[-]</t>
   </si>
   <si>
@@ -203,9 +201,6 @@
     <t>d_z_FW</t>
   </si>
   <si>
-    <t>[N] Norminal vertical load</t>
-  </si>
-  <si>
     <t>[N/m] vertical stiffness</t>
   </si>
   <si>
@@ -239,9 +234,6 @@
     <t>[Ns/m] slip damping</t>
   </si>
   <si>
-    <t>Fz0_RW</t>
-  </si>
-  <si>
     <t>Cy</t>
   </si>
   <si>
@@ -461,12 +453,6 @@
     <t>rebound damping force at 2m/s [N]</t>
   </si>
   <si>
-    <t>F0_suspension_f</t>
-  </si>
-  <si>
-    <t>Preload rear spring [N]</t>
-  </si>
-  <si>
     <t>c_suspension_r</t>
   </si>
   <si>
@@ -479,9 +465,6 @@
     <t>Fd_rebound_r</t>
   </si>
   <si>
-    <t>F0_suspension_r</t>
-  </si>
-  <si>
     <t>compression damping force at 1m/s [N]</t>
   </si>
   <si>
@@ -504,9 +487,6 @@
   </si>
   <si>
     <t>CG_lower_body</t>
-  </si>
-  <si>
-    <t>Preload front spring [N]</t>
   </si>
   <si>
     <t>CG_trim_mass</t>
@@ -548,7 +528,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
@@ -894,11 +874,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:G50"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -925,7 +905,7 @@
     </row>
     <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
@@ -962,7 +942,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B6" s="8">
         <v>-2.3300000000000001E-2</v>
@@ -976,7 +956,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B7" s="8">
         <f>-0.6779+0.364</f>
@@ -1008,7 +988,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B9" s="8">
         <v>0.23532</v>
@@ -1038,7 +1018,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B11" s="8">
         <f>-0.6779+0.549</f>
@@ -1054,7 +1034,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B12" s="8">
         <f>-0.6779+0.487</f>
@@ -1070,7 +1050,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B13" s="8">
         <f>-0.6779+0.539</f>
@@ -1086,7 +1066,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B14" s="8">
         <v>-0.67789999999999995</v>
@@ -1155,7 +1135,7 @@
     </row>
     <row r="19" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B19" s="8">
         <v>0.1883</v>
@@ -1169,7 +1149,7 @@
     </row>
     <row r="20" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B20" s="8">
         <v>0.1883</v>
@@ -1196,7 +1176,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B23" s="8">
         <v>0.35</v>
@@ -1241,7 +1221,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B27" s="8">
         <v>0.12333</v>
@@ -1265,7 +1245,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B29" s="8">
         <v>-8.8999999999999999E-3</v>
@@ -1279,7 +1259,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B30" s="8">
         <v>9.7470000000000001E-2</v>
@@ -1296,12 +1276,12 @@
         <v>9</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B32" s="9">
         <v>2.5000000000000001E-2</v>
@@ -1315,7 +1295,7 @@
     </row>
     <row r="33" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B33" s="9">
         <v>2.5000000000000001E-2</v>
@@ -1382,7 +1362,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B41">
         <f>D3</f>
@@ -1391,7 +1371,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -1399,12 +1379,12 @@
         <v>9</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B45">
         <f>-0.196+0.549</f>
@@ -1420,7 +1400,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B46">
         <f>-0.196</f>
@@ -1436,15 +1416,15 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B47">
-        <v>0.34350000000000003</v>
+        <v>0.31352099999999999</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B48">
         <f>-0.539+0.4946</f>
@@ -1460,7 +1440,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B49">
         <f>-0.539+0.4443</f>
@@ -1476,7 +1456,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B50">
         <f>-0.549+0.3722</f>
@@ -1492,7 +1472,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1500,12 +1480,12 @@
         <v>9</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B54">
         <v>0.29699999999999999</v>
@@ -1513,7 +1493,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B55" s="7">
         <v>9.5000000000000001E-2</v>
@@ -1521,7 +1501,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B56">
         <f>B54-B55</f>
@@ -1530,7 +1510,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B57">
         <f>B41</f>
@@ -1544,7 +1524,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1746,7 +1726,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B9" s="8">
         <v>0</v>
@@ -1772,7 +1752,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8">
@@ -2176,7 +2156,7 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -2286,7 +2266,7 @@
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
@@ -2309,7 +2289,7 @@
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B30">
         <v>14.7</v>
@@ -2335,7 +2315,7 @@
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C31" s="10">
         <v>0.38300000000000001</v>
@@ -2384,11 +2364,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C116"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C114"/>
   <sheetViews>
     <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2404,515 +2384,515 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2">
-        <v>1139.58</v>
-      </c>
-      <c r="C2" t="s">
-        <v>58</v>
+        <v>94</v>
+      </c>
+      <c r="B2" s="4">
+        <v>13.476000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" s="4">
-        <v>13.476000000000001</v>
+        <v>95</v>
+      </c>
+      <c r="B3">
+        <v>11.353999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B4">
-        <v>11.353999999999999</v>
+        <v>1.1231</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B5">
-        <v>1.1231</v>
+        <v>1.6064000000000001</v>
+      </c>
+      <c r="C5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B6">
-        <v>1.6064000000000001</v>
+        <v>1.381</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B7">
-        <v>1.381</v>
+        <v>-4.1430000000000002E-2</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B8">
-        <v>-4.1430000000000002E-2</v>
+        <v>2.63E-2</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B9">
-        <v>2.63E-2</v>
+        <v>0.27056000000000002</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B10">
-        <v>0.27056000000000002</v>
+        <v>-7.6899999999999996E-2</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B11">
-        <v>-7.6899999999999996E-2</v>
+        <v>1.1268</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B12">
-        <v>1.1268</v>
+        <v>25.94</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B13">
-        <v>25.94</v>
+        <v>-4.2329999999999997</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B14">
-        <v>-4.2329999999999997</v>
+        <v>0.33689999999999998</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15">
-        <v>0.33689999999999998</v>
-      </c>
-      <c r="C15" t="s">
-        <v>55</v>
+        <v>97</v>
+      </c>
+      <c r="B15" s="4">
+        <v>7.7855999999999996</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>100</v>
-      </c>
-      <c r="B16" s="4">
-        <v>7.7855999999999996</v>
+        <v>98</v>
+      </c>
+      <c r="B16">
+        <v>8.1697000000000006</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B17">
-        <v>8.1697000000000006</v>
+        <v>-5.9139999999999998E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="B18">
-        <v>-5.9139999999999998E-2</v>
+        <v>1.0532999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>68</v>
       </c>
       <c r="B19">
-        <v>1.0532999999999999</v>
+        <v>0.8327</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B20">
-        <v>0.8327</v>
+        <v>1.3</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B21">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>-1.2556</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B24">
-        <v>-1.2556</v>
+        <v>-3.2067999999999999</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B25">
-        <v>-3.2067999999999999</v>
+        <v>-3.9980000000000002</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B26">
-        <v>-3.9980000000000002</v>
+        <v>22.841000000000001</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B27">
-        <v>22.841000000000001</v>
+        <v>2.1577999999999999</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B28">
-        <v>2.1577999999999999</v>
+        <v>2.5057999999999998</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B29">
-        <v>2.5057999999999998</v>
+        <v>-8.0879999999999994E-2</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B30">
-        <v>-8.0879999999999994E-2</v>
+        <v>-0.22882</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B31">
-        <v>-0.22882</v>
+        <v>0.86765000000000003</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B32">
-        <v>0.86765000000000003</v>
+        <v>0.69677</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B33">
-        <v>0.69677</v>
+        <v>-3.0769999999999999E-2</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B34">
-        <v>-3.0769999999999999E-2</v>
+        <v>-15.815</v>
       </c>
       <c r="C34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="B35">
-        <v>-15.815</v>
-      </c>
-      <c r="C35" t="s">
-        <v>55</v>
+        <v>1.0916999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B36">
-        <v>1.0916999999999999</v>
+        <v>10.486000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B37">
-        <v>10.486000000000001</v>
+        <v>-1.1540000000000001E-3</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B38">
-        <v>-1.1540000000000001E-3</v>
+        <v>-0.68972999999999995</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B39">
-        <v>-0.68972999999999995</v>
+        <v>1.0410999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B40">
-        <v>1.0410999999999999</v>
+        <v>27.445</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B41">
-        <v>27.445</v>
+        <v>-1.0791999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B42">
-        <v>-1.0791999999999999</v>
+        <v>0.19796</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B43">
-        <v>0.19796</v>
+        <v>6.5629999999999994E-2</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B44">
-        <v>6.5629999999999994E-2</v>
+        <v>0.21990000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B45">
-        <v>0.21990000000000001</v>
+        <v>0.21865999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B46">
-        <v>0.21865999999999999</v>
+        <v>0.36820000000000003</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B47">
-        <v>0.36820000000000003</v>
+        <v>0.12180000000000001</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B48">
-        <v>0.12180000000000001</v>
+        <v>0.25439000000000001</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B49">
-        <v>0.25439000000000001</v>
+        <v>-0.17873</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B50">
-        <v>-0.17873</v>
+        <v>-0.91586000000000001</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B51">
-        <v>-0.91586000000000001</v>
+        <v>0.11625000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B52">
-        <v>0.11625000000000001</v>
+        <v>1.4387000000000001</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B53">
-        <v>1.4387000000000001</v>
+        <v>-3.7889999999999998E-3</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B54">
-        <v>-3.7889999999999998E-3</v>
+        <v>-1.5570000000000001E-2</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>122</v>
+        <v>55</v>
       </c>
       <c r="B55">
-        <v>-1.5570000000000001E-2</v>
+        <v>130000</v>
+      </c>
+      <c r="C55" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -2920,584 +2900,562 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>130000</v>
+        <v>800</v>
       </c>
       <c r="C56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="B57">
-        <v>800</v>
+        <v>2</v>
       </c>
       <c r="C57" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>68</v>
-      </c>
-      <c r="B58">
-        <v>2</v>
-      </c>
-      <c r="C58" t="s">
-        <v>69</v>
+      <c r="A58" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
-        <v>61</v>
+      <c r="A59" t="s">
+        <v>94</v>
+      </c>
+      <c r="B59" s="4">
+        <v>13.476000000000001</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="B60">
-        <v>1305.17</v>
-      </c>
-      <c r="C60" t="s">
-        <v>58</v>
+        <v>11.353999999999999</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>97</v>
-      </c>
-      <c r="B61" s="4">
-        <v>13.476000000000001</v>
+        <v>96</v>
+      </c>
+      <c r="B61">
+        <v>1.1231</v>
+      </c>
+      <c r="C61" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B62">
-        <v>11.353999999999999</v>
+        <v>1.6064000000000001</v>
+      </c>
+      <c r="C62" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="B63">
-        <v>1.1231</v>
+        <v>1.355</v>
       </c>
       <c r="C63" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B64">
-        <v>1.6064000000000001</v>
+        <v>-6.0299999999999999E-2</v>
       </c>
       <c r="C64" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B65">
-        <v>1.355</v>
+        <v>2.63E-2</v>
       </c>
       <c r="C65" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B66">
-        <v>-6.0299999999999999E-2</v>
+        <v>0.27056000000000002</v>
       </c>
       <c r="C66" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B67">
-        <v>2.63E-2</v>
+        <v>-7.6899999999999996E-2</v>
       </c>
       <c r="C67" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B68">
-        <v>0.27056000000000002</v>
+        <v>1.1268</v>
       </c>
       <c r="C68" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B69">
-        <v>-7.6899999999999996E-2</v>
+        <v>25.94</v>
       </c>
       <c r="C69" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B70">
-        <v>1.1268</v>
+        <v>-4.2329999999999997</v>
       </c>
       <c r="C70" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B71">
-        <v>25.94</v>
-      </c>
-      <c r="C71" t="s">
-        <v>55</v>
+        <v>0.33689999999999998</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>95</v>
-      </c>
-      <c r="B72">
-        <v>-4.2329999999999997</v>
-      </c>
-      <c r="C72" t="s">
-        <v>55</v>
+        <v>97</v>
+      </c>
+      <c r="B72" s="4">
+        <v>7.7855999999999996</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B73">
-        <v>0.33689999999999998</v>
+        <v>8.1697000000000006</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>100</v>
-      </c>
-      <c r="B74" s="4">
-        <v>7.7855999999999996</v>
+        <v>99</v>
+      </c>
+      <c r="B74">
+        <v>-5.9139999999999998E-2</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="B75">
-        <v>8.1697000000000006</v>
+        <v>1.0532999999999999</v>
+      </c>
+      <c r="C75" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="B76">
-        <v>-5.9139999999999998E-2</v>
+        <v>0.9</v>
+      </c>
+      <c r="C76" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>125</v>
+        <v>69</v>
       </c>
       <c r="B77">
-        <v>1.0532999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="C77" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B78">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="C78" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B79">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="C79" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B80">
-        <v>0</v>
+        <v>-2.2227000000000001</v>
       </c>
       <c r="C80" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B81">
-        <v>0</v>
+        <v>-1.669</v>
       </c>
       <c r="C81" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B82">
-        <v>-2.2227000000000001</v>
+        <v>-4.2880000000000003</v>
       </c>
       <c r="C82" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B83">
-        <v>-1.669</v>
+        <v>15.791</v>
       </c>
       <c r="C83" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B84">
-        <v>-4.2880000000000003</v>
+        <v>1.6935</v>
       </c>
       <c r="C84" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B85">
-        <v>15.791</v>
+        <v>1.4603999999999999</v>
       </c>
       <c r="C85" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B86">
-        <v>1.6935</v>
+        <v>0.66900000000000004</v>
       </c>
       <c r="C86" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B87">
-        <v>1.4603999999999999</v>
+        <v>0.18708</v>
       </c>
       <c r="C87" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B88">
-        <v>0.66900000000000004</v>
+        <v>0.61397000000000002</v>
       </c>
       <c r="C88" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B89">
-        <v>0.18708</v>
+        <v>0.45512000000000002</v>
       </c>
       <c r="C89" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B90">
-        <v>0.61397000000000002</v>
+        <v>1.3292999999999999E-2</v>
       </c>
       <c r="C90" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B91">
-        <v>0.45512000000000002</v>
-      </c>
-      <c r="C91" t="s">
-        <v>55</v>
+        <v>-19.989999999999998</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B92">
-        <v>1.3292999999999999E-2</v>
-      </c>
-      <c r="C92" t="s">
-        <v>55</v>
+        <v>1.3152999999999999</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="B93">
-        <v>-19.989999999999998</v>
+        <v>10.041</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B94">
-        <v>1.3152999999999999</v>
+        <f>-1.61*10^(-8)</f>
+        <v>-1.6100000000000002E-8</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B95">
-        <v>10.041</v>
+        <v>-0.76783999999999997</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
+        <v>104</v>
+      </c>
+      <c r="B96">
+        <v>0.73421999999999998</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>105</v>
       </c>
-      <c r="B96">
-        <f>-1.61*10^(-8)</f>
-        <v>-1.6100000000000002E-8</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
+      <c r="B97">
+        <v>16.39</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>106</v>
       </c>
-      <c r="B97">
-        <v>-0.76783999999999997</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+      <c r="B98">
+        <v>-0.35548999999999997</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>107</v>
       </c>
-      <c r="B98">
-        <v>0.73421999999999998</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
+      <c r="B99">
+        <v>0.26330999999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
         <v>108</v>
       </c>
-      <c r="B99">
-        <v>16.39</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+      <c r="B100">
+        <v>3.0987000000000001E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>109</v>
       </c>
-      <c r="B100">
-        <v>-0.35548999999999997</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
+      <c r="B101">
+        <v>-0.62012999999999996</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>110</v>
       </c>
-      <c r="B101">
-        <v>0.26330999999999999</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
+      <c r="B102">
+        <v>0.98524</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
         <v>111</v>
       </c>
-      <c r="B102">
-        <v>3.0987000000000001E-2</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
+      <c r="B103">
+        <v>0.50453000000000003</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
         <v>112</v>
       </c>
-      <c r="B103">
-        <v>-0.62012999999999996</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
+      <c r="B104">
+        <v>0.36312</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>113</v>
       </c>
-      <c r="B104">
-        <v>0.98524</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
+      <c r="B105">
+        <v>-0.19167999999999999</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
         <v>114</v>
       </c>
-      <c r="B105">
-        <v>0.50453000000000003</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
+      <c r="B106">
+        <v>-0.40709000000000001</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
         <v>115</v>
       </c>
-      <c r="B106">
-        <v>0.36312</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
+      <c r="B107">
+        <v>-0.19924</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
         <v>116</v>
       </c>
-      <c r="B107">
-        <v>-0.19167999999999999</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
+      <c r="B108">
+        <v>-1.7638000000000001E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
         <v>117</v>
       </c>
-      <c r="B108">
-        <v>-0.40709000000000001</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
+      <c r="B109">
+        <v>3.6511</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
         <v>118</v>
       </c>
-      <c r="B109">
-        <v>-0.19924</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
+      <c r="B110">
+        <v>-2.8448000000000001E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
         <v>119</v>
       </c>
-      <c r="B110">
-        <v>-1.7638000000000001E-2</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
+      <c r="B111">
+        <v>-9.8619999999999992E-3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
         <v>120</v>
       </c>
-      <c r="B111">
-        <v>3.6511</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>121</v>
-      </c>
       <c r="B112">
-        <v>-2.8448000000000001E-2</v>
+        <v>141000</v>
+      </c>
+      <c r="C112" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B113">
-        <v>-9.8619999999999992E-3</v>
+        <v>800</v>
+      </c>
+      <c r="C113" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>123</v>
+        <v>66</v>
       </c>
       <c r="B114">
-        <v>141000</v>
+        <v>2</v>
       </c>
       <c r="C114" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>124</v>
-      </c>
-      <c r="B115">
-        <v>800</v>
-      </c>
-      <c r="C115" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>68</v>
-      </c>
-      <c r="B116">
-        <v>2</v>
-      </c>
-      <c r="C116" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -3507,11 +3465,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3549,7 +3507,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B4">
         <v>380</v>
@@ -3560,7 +3518,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B5">
         <v>38416</v>
@@ -3572,7 +3530,7 @@
     </row>
     <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B6" s="10">
         <v>75.8</v>
@@ -3588,7 +3546,7 @@
     </row>
     <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B7" s="10">
         <v>1053.4000000000001</v>
@@ -3631,108 +3589,84 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B11">
         <v>17000</v>
       </c>
       <c r="D11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B12">
         <v>203</v>
       </c>
       <c r="D12" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B13">
         <v>865.8</v>
       </c>
       <c r="D13" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>144</v>
-      </c>
-      <c r="B14">
-        <f>918-43.435+1.666</f>
-        <v>876.23100000000011</v>
-      </c>
-      <c r="D14" t="s">
-        <v>159</v>
+      <c r="A14" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>134</v>
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15">
+        <v>63700</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>141</v>
       </c>
       <c r="B16">
-        <v>63700</v>
-      </c>
-      <c r="C16">
-        <v>20</v>
+        <v>58570</v>
+      </c>
+      <c r="D16" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B17">
-        <v>58570</v>
+        <v>9600</v>
       </c>
       <c r="D17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B18">
-        <v>9600</v>
+        <v>13700</v>
       </c>
       <c r="D18" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>149</v>
-      </c>
-      <c r="B19">
-        <v>13700</v>
-      </c>
-      <c r="D19" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>150</v>
-      </c>
-      <c r="B20">
-        <f>233.88+14.99</f>
-        <v>248.87</v>
-      </c>
-      <c r="D20" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated tire model (dynamic radius takes into account tire compression)
</commit_message>
<xml_diff>
--- a/Data/Data.xlsx
+++ b/Data/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20367"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ga53hon\Desktop\Motorcycle_Dirk_201028\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ga53hon\Documents\motorcycle_model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00A4B2E-6613-43A5-8031-C6822FB43A28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBB34B4-0F28-481D-BD10-C0EBD487EEE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Geometry" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="167">
   <si>
     <t>Group_Frame</t>
   </si>
@@ -523,6 +523,12 @@
   </si>
   <si>
     <t>rider_lean</t>
+  </si>
+  <si>
+    <t>Fz0_FW</t>
+  </si>
+  <si>
+    <t>Fz0_RW</t>
   </si>
 </sst>
 </file>
@@ -877,7 +883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
@@ -2365,10 +2371,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C114"/>
+  <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2382,47 +2388,44 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B2" s="4">
-        <v>13.476000000000001</v>
+    <row r="2" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="10">
+        <v>1100</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B3">
-        <v>11.353999999999999</v>
+        <v>94</v>
+      </c>
+      <c r="B3" s="4">
+        <v>13.476000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B4">
-        <v>1.1231</v>
+        <v>11.353999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="B5">
-        <v>1.6064000000000001</v>
-      </c>
-      <c r="C5" t="s">
-        <v>54</v>
+        <v>1.1231</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6">
-        <v>1.381</v>
+        <v>1.6064000000000001</v>
       </c>
       <c r="C6" t="s">
         <v>54</v>
@@ -2430,10 +2433,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7">
-        <v>-4.1430000000000002E-2</v>
+        <v>1.381</v>
       </c>
       <c r="C7" t="s">
         <v>54</v>
@@ -2441,10 +2444,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8">
-        <v>2.63E-2</v>
+        <v>-4.1430000000000002E-2</v>
       </c>
       <c r="C8" t="s">
         <v>54</v>
@@ -2452,10 +2455,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B9">
-        <v>0.27056000000000002</v>
+        <v>2.63E-2</v>
       </c>
       <c r="C9" t="s">
         <v>54</v>
@@ -2463,10 +2466,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10">
-        <v>-7.6899999999999996E-2</v>
+        <v>0.27056000000000002</v>
       </c>
       <c r="C10" t="s">
         <v>54</v>
@@ -2474,10 +2477,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B11">
-        <v>1.1268</v>
+        <v>-7.6899999999999996E-2</v>
       </c>
       <c r="C11" t="s">
         <v>54</v>
@@ -2485,10 +2488,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B12">
-        <v>25.94</v>
+        <v>1.1268</v>
       </c>
       <c r="C12" t="s">
         <v>54</v>
@@ -2496,10 +2499,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B13">
-        <v>-4.2329999999999997</v>
+        <v>25.94</v>
       </c>
       <c r="C13" t="s">
         <v>54</v>
@@ -2507,10 +2510,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B14">
-        <v>0.33689999999999998</v>
+        <v>-4.2329999999999997</v>
       </c>
       <c r="C14" t="s">
         <v>54</v>
@@ -2518,53 +2521,53 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B15" s="4">
-        <v>7.7855999999999996</v>
+        <v>93</v>
+      </c>
+      <c r="B15">
+        <v>0.33689999999999998</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>98</v>
-      </c>
-      <c r="B16">
-        <v>8.1697000000000006</v>
+        <v>97</v>
+      </c>
+      <c r="B16" s="4">
+        <v>7.7855999999999996</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B17">
-        <v>-5.9139999999999998E-2</v>
+        <v>8.1697000000000006</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="B18">
-        <v>1.0532999999999999</v>
+        <v>-5.9139999999999998E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="B19">
-        <v>0.8327</v>
-      </c>
-      <c r="C19" t="s">
-        <v>54</v>
+        <v>1.0532999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20">
-        <v>1.3</v>
+        <v>0.8327</v>
       </c>
       <c r="C20" t="s">
         <v>54</v>
@@ -2572,10 +2575,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="C21" t="s">
         <v>54</v>
@@ -2583,7 +2586,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -2594,10 +2597,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23">
-        <v>-1.2556</v>
+        <v>0</v>
       </c>
       <c r="C23" t="s">
         <v>54</v>
@@ -2605,10 +2608,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24">
-        <v>-3.2067999999999999</v>
+        <v>-1.2556</v>
       </c>
       <c r="C24" t="s">
         <v>54</v>
@@ -2616,10 +2619,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25">
-        <v>-3.9980000000000002</v>
+        <v>-3.2067999999999999</v>
       </c>
       <c r="C25" t="s">
         <v>54</v>
@@ -2627,10 +2630,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26">
-        <v>22.841000000000001</v>
+        <v>-3.9980000000000002</v>
       </c>
       <c r="C26" t="s">
         <v>54</v>
@@ -2638,10 +2641,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B27">
-        <v>2.1577999999999999</v>
+        <v>22.841000000000001</v>
       </c>
       <c r="C27" t="s">
         <v>54</v>
@@ -2649,10 +2652,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B28">
-        <v>2.5057999999999998</v>
+        <v>2.1577999999999999</v>
       </c>
       <c r="C28" t="s">
         <v>54</v>
@@ -2660,10 +2663,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B29">
-        <v>-8.0879999999999994E-2</v>
+        <v>2.5057999999999998</v>
       </c>
       <c r="C29" t="s">
         <v>54</v>
@@ -2671,10 +2674,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B30">
-        <v>-0.22882</v>
+        <v>-8.0879999999999994E-2</v>
       </c>
       <c r="C30" t="s">
         <v>54</v>
@@ -2682,10 +2685,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B31">
-        <v>0.86765000000000003</v>
+        <v>-0.22882</v>
       </c>
       <c r="C31" t="s">
         <v>54</v>
@@ -2693,10 +2696,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B32">
-        <v>0.69677</v>
+        <v>0.86765000000000003</v>
       </c>
       <c r="C32" t="s">
         <v>54</v>
@@ -2704,10 +2707,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B33">
-        <v>-3.0769999999999999E-2</v>
+        <v>0.69677</v>
       </c>
       <c r="C33" t="s">
         <v>54</v>
@@ -2715,10 +2718,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B34">
-        <v>-15.815</v>
+        <v>-3.0769999999999999E-2</v>
       </c>
       <c r="C34" t="s">
         <v>54</v>
@@ -2726,246 +2729,243 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B35">
-        <v>1.0916999999999999</v>
+        <v>-15.815</v>
+      </c>
+      <c r="C35" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B36">
-        <v>10.486000000000001</v>
+        <v>1.0916999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B37">
-        <v>-1.1540000000000001E-3</v>
+        <v>10.486000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B38">
-        <v>-0.68972999999999995</v>
+        <v>-1.1540000000000001E-3</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B39">
-        <v>1.0410999999999999</v>
+        <v>-0.68972999999999995</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B40">
-        <v>27.445</v>
+        <v>1.0410999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B41">
-        <v>-1.0791999999999999</v>
+        <v>27.445</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B42">
-        <v>0.19796</v>
+        <v>-1.0791999999999999</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B43">
-        <v>6.5629999999999994E-2</v>
+        <v>0.19796</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B44">
-        <v>0.21990000000000001</v>
+        <v>6.5629999999999994E-2</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B45">
-        <v>0.21865999999999999</v>
+        <v>0.21990000000000001</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B46">
-        <v>0.36820000000000003</v>
+        <v>0.21865999999999999</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B47">
-        <v>0.12180000000000001</v>
+        <v>0.36820000000000003</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B48">
-        <v>0.25439000000000001</v>
+        <v>0.12180000000000001</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B49">
-        <v>-0.17873</v>
+        <v>0.25439000000000001</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B50">
-        <v>-0.91586000000000001</v>
+        <v>-0.17873</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B51">
-        <v>0.11625000000000001</v>
+        <v>-0.91586000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B52">
-        <v>1.4387000000000001</v>
+        <v>0.11625000000000001</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B53">
-        <v>-3.7889999999999998E-3</v>
+        <v>1.4387000000000001</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B54">
-        <v>-1.5570000000000001E-2</v>
+        <v>-3.7889999999999998E-3</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>119</v>
       </c>
       <c r="B55">
-        <v>130000</v>
-      </c>
-      <c r="C55" t="s">
-        <v>57</v>
+        <v>-1.5570000000000001E-2</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56">
-        <v>800</v>
+        <v>130000</v>
       </c>
       <c r="C56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>800</v>
+      </c>
+      <c r="C57" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>66</v>
       </c>
-      <c r="B57">
+      <c r="B58">
         <v>2</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>94</v>
-      </c>
-      <c r="B59" s="4">
-        <v>13.476000000000001</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>95</v>
-      </c>
-      <c r="B60">
-        <v>11.353999999999999</v>
+    <row r="60" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B60" s="10">
+        <v>1600</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>96</v>
-      </c>
-      <c r="B61">
-        <v>1.1231</v>
-      </c>
-      <c r="C61" t="s">
-        <v>54</v>
+        <v>94</v>
+      </c>
+      <c r="B61" s="4">
+        <v>13.476000000000001</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B62">
-        <v>1.6064000000000001</v>
-      </c>
-      <c r="C62" t="s">
-        <v>54</v>
+        <v>11.353999999999999</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="B63">
-        <v>1.355</v>
+        <v>1.1231</v>
       </c>
       <c r="C63" t="s">
         <v>54</v>
@@ -2973,10 +2973,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B64">
-        <v>-6.0299999999999999E-2</v>
+        <v>1.6064000000000001</v>
       </c>
       <c r="C64" t="s">
         <v>54</v>
@@ -2984,10 +2984,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B65">
-        <v>2.63E-2</v>
+        <v>1.355</v>
       </c>
       <c r="C65" t="s">
         <v>54</v>
@@ -2995,10 +2995,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B66">
-        <v>0.27056000000000002</v>
+        <v>-6.0299999999999999E-2</v>
       </c>
       <c r="C66" t="s">
         <v>54</v>
@@ -3006,10 +3006,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B67">
-        <v>-7.6899999999999996E-2</v>
+        <v>2.63E-2</v>
       </c>
       <c r="C67" t="s">
         <v>54</v>
@@ -3017,10 +3017,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B68">
-        <v>1.1268</v>
+        <v>0.27056000000000002</v>
       </c>
       <c r="C68" t="s">
         <v>54</v>
@@ -3028,10 +3028,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B69">
-        <v>25.94</v>
+        <v>-7.6899999999999996E-2</v>
       </c>
       <c r="C69" t="s">
         <v>54</v>
@@ -3039,10 +3039,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B70">
-        <v>-4.2329999999999997</v>
+        <v>1.1268</v>
       </c>
       <c r="C70" t="s">
         <v>54</v>
@@ -3050,64 +3050,64 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B71">
-        <v>0.33689999999999998</v>
+        <v>25.94</v>
+      </c>
+      <c r="C71" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>97</v>
-      </c>
-      <c r="B72" s="4">
-        <v>7.7855999999999996</v>
+        <v>92</v>
+      </c>
+      <c r="B72">
+        <v>-4.2329999999999997</v>
+      </c>
+      <c r="C72" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B73">
-        <v>8.1697000000000006</v>
+        <v>0.33689999999999998</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>99</v>
-      </c>
-      <c r="B74">
-        <v>-5.9139999999999998E-2</v>
+        <v>97</v>
+      </c>
+      <c r="B74" s="4">
+        <v>7.7855999999999996</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="B75">
-        <v>1.0532999999999999</v>
-      </c>
-      <c r="C75" t="s">
-        <v>54</v>
+        <v>8.1697000000000006</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="B76">
-        <v>0.9</v>
-      </c>
-      <c r="C76" t="s">
-        <v>54</v>
+        <v>-5.9139999999999998E-2</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>69</v>
+        <v>122</v>
       </c>
       <c r="B77">
-        <v>1.3</v>
+        <v>1.0532999999999999</v>
       </c>
       <c r="C77" t="s">
         <v>54</v>
@@ -3115,10 +3115,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B78">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="C78" t="s">
         <v>54</v>
@@ -3126,10 +3126,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B79">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="C79" t="s">
         <v>54</v>
@@ -3137,10 +3137,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B80">
-        <v>-2.2227000000000001</v>
+        <v>0</v>
       </c>
       <c r="C80" t="s">
         <v>54</v>
@@ -3148,10 +3148,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B81">
-        <v>-1.669</v>
+        <v>0</v>
       </c>
       <c r="C81" t="s">
         <v>54</v>
@@ -3159,10 +3159,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B82">
-        <v>-4.2880000000000003</v>
+        <v>-2.2227000000000001</v>
       </c>
       <c r="C82" t="s">
         <v>54</v>
@@ -3170,10 +3170,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B83">
-        <v>15.791</v>
+        <v>-1.669</v>
       </c>
       <c r="C83" t="s">
         <v>54</v>
@@ -3181,10 +3181,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B84">
-        <v>1.6935</v>
+        <v>-4.2880000000000003</v>
       </c>
       <c r="C84" t="s">
         <v>54</v>
@@ -3192,10 +3192,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B85">
-        <v>1.4603999999999999</v>
+        <v>15.791</v>
       </c>
       <c r="C85" t="s">
         <v>54</v>
@@ -3203,10 +3203,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B86">
-        <v>0.66900000000000004</v>
+        <v>1.6935</v>
       </c>
       <c r="C86" t="s">
         <v>54</v>
@@ -3214,10 +3214,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B87">
-        <v>0.18708</v>
+        <v>1.4603999999999999</v>
       </c>
       <c r="C87" t="s">
         <v>54</v>
@@ -3225,10 +3225,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B88">
-        <v>0.61397000000000002</v>
+        <v>0.66900000000000004</v>
       </c>
       <c r="C88" t="s">
         <v>54</v>
@@ -3236,10 +3236,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B89">
-        <v>0.45512000000000002</v>
+        <v>0.18708</v>
       </c>
       <c r="C89" t="s">
         <v>54</v>
@@ -3247,10 +3247,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B90">
-        <v>1.3292999999999999E-2</v>
+        <v>0.61397000000000002</v>
       </c>
       <c r="C90" t="s">
         <v>54</v>
@@ -3258,203 +3258,225 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B91">
-        <v>-19.989999999999998</v>
+        <v>0.45512000000000002</v>
+      </c>
+      <c r="C91" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="B92">
-        <v>1.3152999999999999</v>
+        <v>1.3292999999999999E-2</v>
+      </c>
+      <c r="C92" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="B93">
-        <v>10.041</v>
+        <v>-19.989999999999998</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
+        <v>100</v>
+      </c>
+      <c r="B94">
+        <v>1.3152999999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>101</v>
+      </c>
+      <c r="B95">
+        <v>10.041</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>102</v>
       </c>
-      <c r="B94">
+      <c r="B96">
         <f>-1.61*10^(-8)</f>
         <v>-1.6100000000000002E-8</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>103</v>
       </c>
-      <c r="B95">
+      <c r="B97">
         <v>-0.76783999999999997</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>104</v>
       </c>
-      <c r="B96">
+      <c r="B98">
         <v>0.73421999999999998</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>105</v>
       </c>
-      <c r="B97">
+      <c r="B99">
         <v>16.39</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
         <v>106</v>
       </c>
-      <c r="B98">
+      <c r="B100">
         <v>-0.35548999999999997</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>107</v>
       </c>
-      <c r="B99">
+      <c r="B101">
         <v>0.26330999999999999</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>108</v>
       </c>
-      <c r="B100">
+      <c r="B102">
         <v>3.0987000000000001E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
         <v>109</v>
       </c>
-      <c r="B101">
+      <c r="B103">
         <v>-0.62012999999999996</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
         <v>110</v>
       </c>
-      <c r="B102">
+      <c r="B104">
         <v>0.98524</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>111</v>
       </c>
-      <c r="B103">
+      <c r="B105">
         <v>0.50453000000000003</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
         <v>112</v>
       </c>
-      <c r="B104">
+      <c r="B106">
         <v>0.36312</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
         <v>113</v>
       </c>
-      <c r="B105">
+      <c r="B107">
         <v>-0.19167999999999999</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
         <v>114</v>
       </c>
-      <c r="B106">
+      <c r="B108">
         <v>-0.40709000000000001</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
         <v>115</v>
       </c>
-      <c r="B107">
+      <c r="B109">
         <v>-0.19924</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
         <v>116</v>
       </c>
-      <c r="B108">
+      <c r="B110">
         <v>-1.7638000000000001E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
         <v>117</v>
       </c>
-      <c r="B109">
+      <c r="B111">
         <v>3.6511</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
         <v>118</v>
       </c>
-      <c r="B110">
+      <c r="B112">
         <v>-2.8448000000000001E-2</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
-        <v>119</v>
-      </c>
-      <c r="B111">
-        <v>-9.8619999999999992E-3</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>120</v>
-      </c>
-      <c r="B112">
-        <v>141000</v>
-      </c>
-      <c r="C112" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B113">
-        <v>800</v>
-      </c>
-      <c r="C113" t="s">
-        <v>58</v>
+        <v>-9.8619999999999992E-3</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
+        <v>120</v>
+      </c>
+      <c r="B114">
+        <v>141000</v>
+      </c>
+      <c r="C114" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>121</v>
+      </c>
+      <c r="B115">
+        <v>800</v>
+      </c>
+      <c r="C115" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
         <v>66</v>
       </c>
-      <c r="B114">
+      <c r="B116">
         <v>2</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C116" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>